<commit_message>
Complete repository refresh - remove all files and re-add to force clean rebuild
</commit_message>
<xml_diff>
--- a/data_raw/serie_semanal_ingreso_medio_exportacion_inac.xlsx
+++ b/data_raw/serie_semanal_ingreso_medio_exportacion_inac.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Datos y Estadísticas\Publicaciones Web\Públicos\Boletín Semanal\Salidas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\inac.local\archivos\GIF\Datos y Estadísticas\Publicaciones Web\Públicos\Boletín Semanal\Salidas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E910552-9D2F-4E8B-96EF-1120699A050A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6B11AD-E333-4194-925B-E30830FBE961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INAC" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
     <xf numFmtId="43" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -511,7 +511,6 @@
     <xf numFmtId="14" fontId="21" fillId="2" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="9" xfId="39" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="Columnas2" xfId="24" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -808,13 +807,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W1263"/>
+  <dimension ref="A1:W1265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B1246" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B1258" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="F1270" sqref="F1270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -925,7 +924,7 @@
       </c>
       <c r="B5" s="35">
         <f ca="1">TODAY()</f>
-        <v>46043</v>
+        <v>46057</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -53496,7 +53495,7 @@
       </c>
     </row>
     <row r="1158" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1158" s="40">
+      <c r="A1158" s="24">
         <v>45304</v>
       </c>
       <c r="B1158" s="13">
@@ -53534,7 +53533,7 @@
       </c>
     </row>
     <row r="1159" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1159" s="40">
+      <c r="A1159" s="24">
         <v>45311</v>
       </c>
       <c r="B1159" s="13">
@@ -53572,7 +53571,7 @@
       </c>
     </row>
     <row r="1160" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1160" s="40">
+      <c r="A1160" s="24">
         <v>45318</v>
       </c>
       <c r="B1160" s="13">
@@ -53610,7 +53609,7 @@
       </c>
     </row>
     <row r="1161" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1161" s="40">
+      <c r="A1161" s="24">
         <v>45325</v>
       </c>
       <c r="B1161" s="13">
@@ -53648,7 +53647,7 @@
       </c>
     </row>
     <row r="1162" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1162" s="40">
+      <c r="A1162" s="24">
         <v>45332</v>
       </c>
       <c r="B1162" s="13">
@@ -53686,7 +53685,7 @@
       </c>
     </row>
     <row r="1163" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1163" s="40">
+      <c r="A1163" s="24">
         <v>45339</v>
       </c>
       <c r="B1163" s="13">
@@ -53724,7 +53723,7 @@
       </c>
     </row>
     <row r="1164" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1164" s="40">
+      <c r="A1164" s="24">
         <v>45346</v>
       </c>
       <c r="B1164" s="13">
@@ -53762,7 +53761,7 @@
       </c>
     </row>
     <row r="1165" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1165" s="40">
+      <c r="A1165" s="24">
         <v>45353</v>
       </c>
       <c r="B1165" s="13">
@@ -53787,7 +53786,7 @@
         <v>3930.3634262421583</v>
       </c>
       <c r="I1165" s="14">
-        <v>3575.1060841405906</v>
+        <v>3575.1060841405902</v>
       </c>
       <c r="J1165" s="13">
         <v>4062.5365999999999</v>
@@ -53800,7 +53799,7 @@
       </c>
     </row>
     <row r="1166" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1166" s="40">
+      <c r="A1166" s="24">
         <v>45360</v>
       </c>
       <c r="B1166" s="13">
@@ -53838,7 +53837,7 @@
       </c>
     </row>
     <row r="1167" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1167" s="40">
+      <c r="A1167" s="24">
         <v>45367</v>
       </c>
       <c r="B1167" s="13">
@@ -53876,7 +53875,7 @@
       </c>
     </row>
     <row r="1168" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1168" s="40">
+      <c r="A1168" s="24">
         <v>45374</v>
       </c>
       <c r="B1168" s="13">
@@ -53914,7 +53913,7 @@
       </c>
     </row>
     <row r="1169" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1169" s="40">
+      <c r="A1169" s="24">
         <v>45381</v>
       </c>
       <c r="B1169" s="13">
@@ -53952,7 +53951,7 @@
       </c>
     </row>
     <row r="1170" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1170" s="40">
+      <c r="A1170" s="24">
         <v>45388</v>
       </c>
       <c r="B1170" s="13">
@@ -53990,7 +53989,7 @@
       </c>
     </row>
     <row r="1171" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1171" s="40">
+      <c r="A1171" s="24">
         <v>45395</v>
       </c>
       <c r="B1171" s="13">
@@ -54028,7 +54027,7 @@
       </c>
     </row>
     <row r="1172" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1172" s="40">
+      <c r="A1172" s="24">
         <v>45402</v>
       </c>
       <c r="B1172" s="13">
@@ -54066,7 +54065,7 @@
       </c>
     </row>
     <row r="1173" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1173" s="40">
+      <c r="A1173" s="24">
         <v>45409</v>
       </c>
       <c r="B1173" s="13">
@@ -54079,7 +54078,7 @@
         <v>3743.1898864551076</v>
       </c>
       <c r="E1173" s="14">
-        <v>3843.0171122321035</v>
+        <v>3843.0171122321044</v>
       </c>
       <c r="F1173" s="13">
         <v>691.08130000000006</v>
@@ -54104,7 +54103,7 @@
       </c>
     </row>
     <row r="1174" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1174" s="40">
+      <c r="A1174" s="24">
         <v>45416</v>
       </c>
       <c r="B1174" s="13">
@@ -54117,7 +54116,7 @@
         <v>4351.7719768865618</v>
       </c>
       <c r="E1174" s="14">
-        <v>3939.3430114280163</v>
+        <v>3939.3430114280172</v>
       </c>
       <c r="F1174" s="13">
         <v>625.44079999999997</v>
@@ -54142,7 +54141,7 @@
       </c>
     </row>
     <row r="1175" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1175" s="40">
+      <c r="A1175" s="24">
         <v>45423</v>
       </c>
       <c r="B1175" s="13">
@@ -54155,7 +54154,7 @@
         <v>4151.5723390857438</v>
       </c>
       <c r="E1175" s="14">
-        <v>3955.4372729635274</v>
+        <v>3955.4372729635284</v>
       </c>
       <c r="F1175" s="13">
         <v>1393.8427999999999</v>
@@ -54180,7 +54179,7 @@
       </c>
     </row>
     <row r="1176" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1176" s="40">
+      <c r="A1176" s="24">
         <v>45430</v>
       </c>
       <c r="B1176" s="13">
@@ -54218,7 +54217,7 @@
       </c>
     </row>
     <row r="1177" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1177" s="40">
+      <c r="A1177" s="24">
         <v>45437</v>
       </c>
       <c r="B1177" s="13">
@@ -54256,7 +54255,7 @@
       </c>
     </row>
     <row r="1178" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1178" s="40">
+      <c r="A1178" s="24">
         <v>45444</v>
       </c>
       <c r="B1178" s="13">
@@ -54294,7 +54293,7 @@
       </c>
     </row>
     <row r="1179" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1179" s="40">
+      <c r="A1179" s="24">
         <v>45451</v>
       </c>
       <c r="B1179" s="13">
@@ -54332,7 +54331,7 @@
       </c>
     </row>
     <row r="1180" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1180" s="40">
+      <c r="A1180" s="24">
         <v>45458</v>
       </c>
       <c r="B1180" s="13">
@@ -54370,7 +54369,7 @@
       </c>
     </row>
     <row r="1181" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1181" s="40">
+      <c r="A1181" s="24">
         <v>45465</v>
       </c>
       <c r="B1181" s="13">
@@ -54408,7 +54407,7 @@
       </c>
     </row>
     <row r="1182" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1182" s="40">
+      <c r="A1182" s="24">
         <v>45472</v>
       </c>
       <c r="B1182" s="13">
@@ -54446,7 +54445,7 @@
       </c>
     </row>
     <row r="1183" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1183" s="40">
+      <c r="A1183" s="24">
         <v>45479</v>
       </c>
       <c r="B1183" s="13">
@@ -54484,7 +54483,7 @@
       </c>
     </row>
     <row r="1184" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1184" s="40">
+      <c r="A1184" s="24">
         <v>45486</v>
       </c>
       <c r="B1184" s="13">
@@ -54522,7 +54521,7 @@
       </c>
     </row>
     <row r="1185" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1185" s="40">
+      <c r="A1185" s="24">
         <v>45493</v>
       </c>
       <c r="B1185" s="13">
@@ -54547,7 +54546,7 @@
         <v>4503.2383558639631</v>
       </c>
       <c r="I1185" s="14">
-        <v>4446.3732870828371</v>
+        <v>4446.3732870828389</v>
       </c>
       <c r="J1185" s="13">
         <v>3367.5416</v>
@@ -54560,7 +54559,7 @@
       </c>
     </row>
     <row r="1186" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1186" s="40">
+      <c r="A1186" s="24">
         <v>45500</v>
       </c>
       <c r="B1186" s="13">
@@ -54598,7 +54597,7 @@
       </c>
     </row>
     <row r="1187" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1187" s="40">
+      <c r="A1187" s="24">
         <v>45507</v>
       </c>
       <c r="B1187" s="13">
@@ -54636,7 +54635,7 @@
       </c>
     </row>
     <row r="1188" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1188" s="40">
+      <c r="A1188" s="24">
         <v>45514</v>
       </c>
       <c r="B1188" s="13">
@@ -54674,7 +54673,7 @@
       </c>
     </row>
     <row r="1189" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1189" s="40">
+      <c r="A1189" s="24">
         <v>45521</v>
       </c>
       <c r="B1189" s="13">
@@ -54712,7 +54711,7 @@
       </c>
     </row>
     <row r="1190" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1190" s="40">
+      <c r="A1190" s="24">
         <v>45528</v>
       </c>
       <c r="B1190" s="13">
@@ -54750,7 +54749,7 @@
       </c>
     </row>
     <row r="1191" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1191" s="40">
+      <c r="A1191" s="24">
         <v>45535</v>
       </c>
       <c r="B1191" s="13">
@@ -54788,7 +54787,7 @@
       </c>
     </row>
     <row r="1192" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1192" s="40">
+      <c r="A1192" s="24">
         <v>45542</v>
       </c>
       <c r="B1192" s="13">
@@ -54801,7 +54800,7 @@
         <v>3714.6529959308918</v>
       </c>
       <c r="E1192" s="14">
-        <v>4249.8371965672723</v>
+        <v>4249.8371965672713</v>
       </c>
       <c r="F1192" s="13">
         <v>915.8922</v>
@@ -54826,7 +54825,7 @@
       </c>
     </row>
     <row r="1193" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1193" s="40">
+      <c r="A1193" s="24">
         <v>45549</v>
       </c>
       <c r="B1193" s="13">
@@ -54864,7 +54863,7 @@
       </c>
     </row>
     <row r="1194" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1194" s="40">
+      <c r="A1194" s="24">
         <v>45556</v>
       </c>
       <c r="B1194" s="13">
@@ -54902,7 +54901,7 @@
       </c>
     </row>
     <row r="1195" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1195" s="40">
+      <c r="A1195" s="24">
         <v>45563</v>
       </c>
       <c r="B1195" s="13">
@@ -54940,7 +54939,7 @@
       </c>
     </row>
     <row r="1196" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1196" s="40">
+      <c r="A1196" s="24">
         <v>45570</v>
       </c>
       <c r="B1196" s="13">
@@ -54978,7 +54977,7 @@
       </c>
     </row>
     <row r="1197" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1197" s="40">
+      <c r="A1197" s="24">
         <v>45577</v>
       </c>
       <c r="B1197" s="13">
@@ -55016,7 +55015,7 @@
       </c>
     </row>
     <row r="1198" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1198" s="40">
+      <c r="A1198" s="24">
         <v>45584</v>
       </c>
       <c r="B1198" s="13">
@@ -55054,7 +55053,7 @@
       </c>
     </row>
     <row r="1199" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1199" s="40">
+      <c r="A1199" s="24">
         <v>45591</v>
       </c>
       <c r="B1199" s="13">
@@ -55067,7 +55066,7 @@
         <v>4811.1216968574927</v>
       </c>
       <c r="E1199" s="14">
-        <v>4410.8853143259794</v>
+        <v>4410.8853143259776</v>
       </c>
       <c r="F1199" s="13">
         <v>923.27440000000001</v>
@@ -55092,7 +55091,7 @@
       </c>
     </row>
     <row r="1200" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1200" s="40">
+      <c r="A1200" s="24">
         <v>45598</v>
       </c>
       <c r="B1200" s="13">
@@ -55130,7 +55129,7 @@
       </c>
     </row>
     <row r="1201" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1201" s="40">
+      <c r="A1201" s="24">
         <v>45605</v>
       </c>
       <c r="B1201" s="13">
@@ -55168,7 +55167,7 @@
       </c>
     </row>
     <row r="1202" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1202" s="40">
+      <c r="A1202" s="24">
         <v>45612</v>
       </c>
       <c r="B1202" s="13">
@@ -55206,7 +55205,7 @@
       </c>
     </row>
     <row r="1203" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1203" s="40">
+      <c r="A1203" s="24">
         <v>45619</v>
       </c>
       <c r="B1203" s="13">
@@ -55244,7 +55243,7 @@
       </c>
     </row>
     <row r="1204" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1204" s="40">
+      <c r="A1204" s="24">
         <v>45626</v>
       </c>
       <c r="B1204" s="13">
@@ -55282,7 +55281,7 @@
       </c>
     </row>
     <row r="1205" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1205" s="40">
+      <c r="A1205" s="24">
         <v>45633</v>
       </c>
       <c r="B1205" s="13">
@@ -55320,7 +55319,7 @@
       </c>
     </row>
     <row r="1206" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1206" s="40">
+      <c r="A1206" s="24">
         <v>45640</v>
       </c>
       <c r="B1206" s="13">
@@ -55358,7 +55357,7 @@
       </c>
     </row>
     <row r="1207" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1207" s="40">
+      <c r="A1207" s="24">
         <v>45647</v>
       </c>
       <c r="B1207" s="13">
@@ -55371,7 +55370,7 @@
         <v>4252.7279635792374</v>
       </c>
       <c r="E1207" s="14">
-        <v>4389.4044684956052</v>
+        <v>4389.4044684956043</v>
       </c>
       <c r="F1207" s="13">
         <v>1109.1464000000001</v>
@@ -55383,7 +55382,7 @@
         <v>4145.9867547787508</v>
       </c>
       <c r="I1207" s="14">
-        <v>4315.8033455629657</v>
+        <v>4315.8033455629666</v>
       </c>
       <c r="J1207" s="13">
         <v>8213.6905999999999</v>
@@ -55396,7 +55395,7 @@
       </c>
     </row>
     <row r="1208" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1208" s="40">
+      <c r="A1208" s="24">
         <v>45654</v>
       </c>
       <c r="B1208" s="13">
@@ -55421,7 +55420,7 @@
         <v>4947.3851972485918</v>
       </c>
       <c r="I1208" s="14">
-        <v>4350.8974691131998</v>
+        <v>4350.8974691132007</v>
       </c>
       <c r="J1208" s="13">
         <v>9287.4572000000007</v>
@@ -55434,20 +55433,20 @@
       </c>
     </row>
     <row r="1209" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1209" s="40">
+      <c r="A1209" s="24">
         <v>45661</v>
       </c>
       <c r="B1209" s="13">
-        <v>40002.602200000001</v>
+        <v>40002.254699999998</v>
       </c>
       <c r="C1209" s="13">
         <v>8227.7469000000001</v>
       </c>
       <c r="D1209" s="13">
-        <v>4861.9145297238056</v>
+        <v>4861.8722945889349</v>
       </c>
       <c r="E1209" s="14">
-        <v>4603.9607457779821</v>
+        <v>4603.9520191017509</v>
       </c>
       <c r="F1209" s="13">
         <v>2751.9634000000001</v>
@@ -55468,11 +55467,11 @@
       <c r="L1209" s="13"/>
       <c r="M1209" s="13"/>
       <c r="N1209" s="15">
-        <v>49129.5648</v>
+        <v>49129.217299999997</v>
       </c>
     </row>
     <row r="1210" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1210" s="40">
+      <c r="A1210" s="24">
         <v>45668</v>
       </c>
       <c r="B1210" s="13">
@@ -55485,7 +55484,7 @@
         <v>4532.4957847164742</v>
       </c>
       <c r="E1210" s="14">
-        <v>4508.6407084191396</v>
+        <v>4508.6319604314422</v>
       </c>
       <c r="F1210" s="13">
         <v>1813.4111</v>
@@ -55497,7 +55496,7 @@
         <v>6882.5719118850975</v>
       </c>
       <c r="I1210" s="14">
-        <v>5131.0721532756534</v>
+        <v>5131.0721532756543</v>
       </c>
       <c r="J1210" s="13">
         <v>5833.4898999999996</v>
@@ -55510,7 +55509,7 @@
       </c>
     </row>
     <row r="1211" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1211" s="40">
+      <c r="A1211" s="24">
         <v>45675</v>
       </c>
       <c r="B1211" s="13">
@@ -55523,7 +55522,7 @@
         <v>4637.0540275804779</v>
       </c>
       <c r="E1211" s="14">
-        <v>4537.1224422857194</v>
+        <v>4537.1133140358179</v>
       </c>
       <c r="F1211" s="13">
         <v>1790.9604999999999</v>
@@ -55535,7 +55534,7 @@
         <v>6099.4532507976128</v>
       </c>
       <c r="I1211" s="14">
-        <v>5615.5313175907377</v>
+        <v>5615.5313175907386</v>
       </c>
       <c r="J1211" s="13">
         <v>4923.6122999999998</v>
@@ -55548,7 +55547,7 @@
       </c>
     </row>
     <row r="1212" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1212" s="40">
+      <c r="A1212" s="24">
         <v>45682</v>
       </c>
       <c r="B1212" s="13">
@@ -55561,7 +55560,7 @@
         <v>4833.6383582173466</v>
       </c>
       <c r="E1212" s="14">
-        <v>4670.5531126860587</v>
+        <v>4670.5434936426145</v>
       </c>
       <c r="F1212" s="13">
         <v>1637.0943</v>
@@ -55586,7 +55585,7 @@
       </c>
     </row>
     <row r="1213" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1213" s="40">
+      <c r="A1213" s="24">
         <v>45689</v>
       </c>
       <c r="B1213" s="13">
@@ -55599,7 +55598,7 @@
         <v>4746.7946040659472</v>
       </c>
       <c r="E1213" s="14">
-        <v>4691.5092465550088</v>
+        <v>4691.500419453695</v>
       </c>
       <c r="F1213" s="13">
         <v>2092.5389</v>
@@ -55624,7 +55623,7 @@
       </c>
     </row>
     <row r="1214" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1214" s="40">
+      <c r="A1214" s="24">
         <v>45696</v>
       </c>
       <c r="B1214" s="13">
@@ -55649,7 +55648,7 @@
         <v>5483.9420094229508</v>
       </c>
       <c r="I1214" s="14">
-        <v>5618.8491234155317</v>
+        <v>5618.8491234155326</v>
       </c>
       <c r="J1214" s="13">
         <v>8807.2849999999999</v>
@@ -55662,7 +55661,7 @@
       </c>
     </row>
     <row r="1215" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1215" s="40">
+      <c r="A1215" s="24">
         <v>45703</v>
       </c>
       <c r="B1215" s="13">
@@ -55700,7 +55699,7 @@
       </c>
     </row>
     <row r="1216" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1216" s="40">
+      <c r="A1216" s="24">
         <v>45710</v>
       </c>
       <c r="B1216" s="13">
@@ -55725,7 +55724,7 @@
         <v>4337.7130954170489</v>
       </c>
       <c r="I1216" s="14">
-        <v>4764.4312599888553</v>
+        <v>4764.4312599888563</v>
       </c>
       <c r="J1216" s="13">
         <v>3920.1588999999999</v>
@@ -55738,7 +55737,7 @@
       </c>
     </row>
     <row r="1217" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1217" s="40">
+      <c r="A1217" s="24">
         <v>45717</v>
       </c>
       <c r="B1217" s="13">
@@ -55776,7 +55775,7 @@
       </c>
     </row>
     <row r="1218" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1218" s="40">
+      <c r="A1218" s="24">
         <v>45724</v>
       </c>
       <c r="B1218" s="13">
@@ -55814,7 +55813,7 @@
       </c>
     </row>
     <row r="1219" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1219" s="40">
+      <c r="A1219" s="24">
         <v>45731</v>
       </c>
       <c r="B1219" s="13">
@@ -55827,7 +55826,7 @@
         <v>4760.4158560393298</v>
       </c>
       <c r="E1219" s="14">
-        <v>4756.3449304404712</v>
+        <v>4756.3449304404703</v>
       </c>
       <c r="F1219" s="13">
         <v>1866.9058</v>
@@ -55852,7 +55851,7 @@
       </c>
     </row>
     <row r="1220" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1220" s="40">
+      <c r="A1220" s="24">
         <v>45738</v>
       </c>
       <c r="B1220" s="13">
@@ -55890,7 +55889,7 @@
       </c>
     </row>
     <row r="1221" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1221" s="40">
+      <c r="A1221" s="24">
         <v>45745</v>
       </c>
       <c r="B1221" s="13">
@@ -55903,7 +55902,7 @@
         <v>4701.8076037281035</v>
       </c>
       <c r="E1221" s="14">
-        <v>4670.5473471968171</v>
+        <v>4670.547347196818</v>
       </c>
       <c r="F1221" s="13">
         <v>673.16070000000002</v>
@@ -55928,20 +55927,20 @@
       </c>
     </row>
     <row r="1222" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1222" s="40">
+      <c r="A1222" s="24">
         <v>45752</v>
       </c>
       <c r="B1222" s="13">
-        <v>48560.4133</v>
+        <v>48559.015899999999</v>
       </c>
       <c r="C1222" s="13">
         <v>10009.820100000001</v>
       </c>
       <c r="D1222" s="13">
-        <v>4851.2773271519627</v>
+        <v>4851.1377242434155</v>
       </c>
       <c r="E1222" s="14">
-        <v>4696.0209934111472</v>
+        <v>4695.9889906735043</v>
       </c>
       <c r="F1222" s="13">
         <v>1081.6878999999999</v>
@@ -55962,11 +55961,11 @@
       <c r="L1222" s="13"/>
       <c r="M1222" s="13"/>
       <c r="N1222" s="15">
-        <v>52982.040799999995</v>
+        <v>52980.643399999994</v>
       </c>
     </row>
     <row r="1223" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1223" s="40">
+      <c r="A1223" s="24">
         <v>45759</v>
       </c>
       <c r="B1223" s="13">
@@ -55979,7 +55978,7 @@
         <v>4613.3343787360272</v>
       </c>
       <c r="E1223" s="14">
-        <v>4695.6837942773263</v>
+        <v>4695.6528467809921</v>
       </c>
       <c r="F1223" s="13">
         <v>1661.2738999999999</v>
@@ -56004,7 +56003,7 @@
       </c>
     </row>
     <row r="1224" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1224" s="40">
+      <c r="A1224" s="24">
         <v>45766</v>
       </c>
       <c r="B1224" s="13">
@@ -56017,7 +56016,7 @@
         <v>4504.1722018570981</v>
       </c>
       <c r="E1224" s="14">
-        <v>4673.3652771652705</v>
+        <v>4673.3313732946226</v>
       </c>
       <c r="F1224" s="13">
         <v>678.69989999999996</v>
@@ -56042,20 +56041,20 @@
       </c>
     </row>
     <row r="1225" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1225" s="40">
+      <c r="A1225" s="24">
         <v>45773</v>
       </c>
       <c r="B1225" s="13">
-        <v>55231.831200000001</v>
+        <v>55124.155200000001</v>
       </c>
       <c r="C1225" s="13">
-        <v>10535.945400000001</v>
+        <v>10498.2588</v>
       </c>
       <c r="D1225" s="13">
-        <v>5242.2283053972551</v>
+        <v>5250.790273907136</v>
       </c>
       <c r="E1225" s="14">
-        <v>4737.088282566523</v>
+        <v>4738.7543938000908</v>
       </c>
       <c r="F1225" s="13">
         <v>723.6875</v>
@@ -56076,11 +56075,11 @@
       <c r="L1225" s="13"/>
       <c r="M1225" s="13"/>
       <c r="N1225" s="15">
-        <v>64316.346000000005</v>
+        <v>64208.67</v>
       </c>
     </row>
     <row r="1226" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1226" s="40">
+      <c r="A1226" s="24">
         <v>45780</v>
       </c>
       <c r="B1226" s="13">
@@ -56093,7 +56092,7 @@
         <v>4813.0204026457086</v>
       </c>
       <c r="E1226" s="14">
-        <v>4820.1307322024177</v>
+        <v>4821.9812675094718</v>
       </c>
       <c r="F1226" s="13">
         <v>823.7826</v>
@@ -56118,7 +56117,7 @@
       </c>
     </row>
     <row r="1227" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1227" s="40">
+      <c r="A1227" s="24">
         <v>45787</v>
       </c>
       <c r="B1227" s="13">
@@ -56131,7 +56130,7 @@
         <v>4954.3026679431059</v>
       </c>
       <c r="E1227" s="14">
-        <v>4888.8948939701686</v>
+        <v>4890.6111910146301</v>
       </c>
       <c r="F1227" s="13">
         <v>699.97680000000003</v>
@@ -56156,7 +56155,7 @@
       </c>
     </row>
     <row r="1228" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1228" s="40">
+      <c r="A1228" s="24">
         <v>45794</v>
       </c>
       <c r="B1228" s="13">
@@ -56169,7 +56168,7 @@
         <v>5174.2919588572313</v>
       </c>
       <c r="E1228" s="14">
-        <v>5046.8130108503183</v>
+        <v>5048.416067317241</v>
       </c>
       <c r="F1228" s="13">
         <v>677.62339999999995</v>
@@ -56194,7 +56193,7 @@
       </c>
     </row>
     <row r="1229" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1229" s="40">
+      <c r="A1229" s="24">
         <v>45801</v>
       </c>
       <c r="B1229" s="13">
@@ -56207,7 +56206,7 @@
         <v>5128.5357907447842</v>
       </c>
       <c r="E1229" s="14">
-        <v>4982.5589321239358</v>
+        <v>4984.0678413824007</v>
       </c>
       <c r="F1229" s="13">
         <v>465.10070000000002</v>
@@ -56232,7 +56231,7 @@
       </c>
     </row>
     <row r="1230" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1230" s="40">
+      <c r="A1230" s="24">
         <v>45808</v>
       </c>
       <c r="B1230" s="13">
@@ -56270,7 +56269,7 @@
       </c>
     </row>
     <row r="1231" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1231" s="40">
+      <c r="A1231" s="24">
         <v>45815</v>
       </c>
       <c r="B1231" s="13">
@@ -56308,20 +56307,20 @@
       </c>
     </row>
     <row r="1232" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1232" s="40">
+      <c r="A1232" s="24">
         <v>45822</v>
       </c>
       <c r="B1232" s="13">
-        <v>55040.699200000003</v>
+        <v>55038.055200000003</v>
       </c>
       <c r="C1232" s="13">
         <v>11413.672200000001</v>
       </c>
       <c r="D1232" s="13">
-        <v>4822.347990684365</v>
+        <v>4822.1163386837061</v>
       </c>
       <c r="E1232" s="14">
-        <v>4910.155913535913</v>
+        <v>4910.1042400789902</v>
       </c>
       <c r="F1232" s="13">
         <v>1933.1436000000001</v>
@@ -56342,11 +56341,11 @@
       <c r="L1232" s="13"/>
       <c r="M1232" s="13"/>
       <c r="N1232" s="15">
-        <v>68157.372999999992</v>
+        <v>68154.728999999992</v>
       </c>
     </row>
     <row r="1233" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1233" s="40">
+      <c r="A1233" s="24">
         <v>45829</v>
       </c>
       <c r="B1233" s="13">
@@ -56359,7 +56358,7 @@
         <v>4913.7441789882268</v>
       </c>
       <c r="E1233" s="14">
-        <v>4836.5248348711239</v>
+        <v>4836.469487737555</v>
       </c>
       <c r="F1233" s="13">
         <v>910.61059999999998</v>
@@ -56384,7 +56383,7 @@
       </c>
     </row>
     <row r="1234" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1234" s="40">
+      <c r="A1234" s="24">
         <v>45836</v>
       </c>
       <c r="B1234" s="13">
@@ -56397,7 +56396,7 @@
         <v>4900.5613652109014</v>
       </c>
       <c r="E1234" s="14">
-        <v>4766.4406933790788</v>
+        <v>4766.381961573491</v>
       </c>
       <c r="F1234" s="13">
         <v>556.48080000000004</v>
@@ -56409,7 +56408,7 @@
         <v>6232.9559455378785</v>
       </c>
       <c r="I1234" s="14">
-        <v>6273.3822151253544</v>
+        <v>6273.3822151253535</v>
       </c>
       <c r="J1234" s="13">
         <v>8405.0920000000006</v>
@@ -56422,20 +56421,20 @@
       </c>
     </row>
     <row r="1235" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1235" s="40">
+      <c r="A1235" s="24">
         <v>45843</v>
       </c>
       <c r="B1235" s="13">
-        <v>72127.169500000004</v>
+        <v>72125.569600000003</v>
       </c>
       <c r="C1235" s="13">
         <v>14071.575000000001</v>
       </c>
       <c r="D1235" s="13">
-        <v>5125.7353565610101</v>
+        <v>5125.621659266998</v>
       </c>
       <c r="E1235" s="14">
-        <v>4955.5183591622945</v>
+        <v>4955.4276592396536</v>
       </c>
       <c r="F1235" s="13">
         <v>1182.9712999999999</v>
@@ -56447,7 +56446,7 @@
         <v>5270.8131997196551</v>
       </c>
       <c r="I1235" s="14">
-        <v>6279.4686229430436</v>
+        <v>6279.4686229430445</v>
       </c>
       <c r="J1235" s="13">
         <v>12601.2554</v>
@@ -56456,24 +56455,24 @@
       <c r="L1235" s="13"/>
       <c r="M1235" s="13"/>
       <c r="N1235" s="15">
-        <v>85911.396200000003</v>
+        <v>85909.796300000002</v>
       </c>
     </row>
     <row r="1236" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1236" s="40">
+      <c r="A1236" s="24">
         <v>45850</v>
       </c>
       <c r="B1236" s="13">
         <v>38590.557000000001</v>
       </c>
       <c r="C1236" s="13">
-        <v>8634.5427</v>
+        <v>8635.1026999999995</v>
       </c>
       <c r="D1236" s="13">
-        <v>4469.3226197144177</v>
+        <v>4469.0327771087195</v>
       </c>
       <c r="E1236" s="14">
-        <v>4833.7213031073743</v>
+        <v>4833.627777242179</v>
       </c>
       <c r="F1236" s="13">
         <v>509.77510000000001</v>
@@ -56498,7 +56497,7 @@
       </c>
     </row>
     <row r="1237" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1237" s="40">
+      <c r="A1237" s="24">
         <v>45857</v>
       </c>
       <c r="B1237" s="13">
@@ -56511,7 +56510,7 @@
         <v>5279.8066063917322</v>
       </c>
       <c r="E1237" s="14">
-        <v>4927.494506071961</v>
+        <v>4927.3911159242625</v>
       </c>
       <c r="F1237" s="13">
         <v>770.73030000000006</v>
@@ -56536,7 +56535,7 @@
       </c>
     </row>
     <row r="1238" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1238" s="40">
+      <c r="A1238" s="24">
         <v>45864</v>
       </c>
       <c r="B1238" s="13">
@@ -56549,7 +56548,7 @@
         <v>5523.9290394646114</v>
       </c>
       <c r="E1238" s="14">
-        <v>5022.115350046427</v>
+        <v>5022.0176430942774</v>
       </c>
       <c r="F1238" s="13">
         <v>937.15679999999998</v>
@@ -56564,17 +56563,17 @@
         <v>5662.7424793253513</v>
       </c>
       <c r="J1238" s="13">
-        <v>4867.1611000000003</v>
+        <v>5018.8672999999999</v>
       </c>
       <c r="K1238" s="13"/>
       <c r="L1238" s="13"/>
       <c r="M1238" s="13"/>
       <c r="N1238" s="15">
-        <v>53578.999799999998</v>
+        <v>53730.705999999998</v>
       </c>
     </row>
     <row r="1239" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1239" s="40">
+      <c r="A1239" s="24">
         <v>45871</v>
       </c>
       <c r="B1239" s="13">
@@ -56587,7 +56586,7 @@
         <v>5020.1039422361791</v>
       </c>
       <c r="E1239" s="14">
-        <v>4984.1237231395626</v>
+        <v>4984.0247080089212</v>
       </c>
       <c r="F1239" s="13">
         <v>1951.8497</v>
@@ -56599,45 +56598,45 @@
         <v>6823.3180379492396</v>
       </c>
       <c r="I1239" s="14">
-        <v>6067.7529720316115</v>
+        <v>6067.7529720316088</v>
       </c>
       <c r="J1239" s="13">
-        <v>8231.3942999999999</v>
+        <v>8211.3163000000004</v>
       </c>
       <c r="K1239" s="13"/>
       <c r="L1239" s="13"/>
       <c r="M1239" s="13"/>
       <c r="N1239" s="15">
-        <v>65181.032899999998</v>
+        <v>65160.954899999997</v>
       </c>
     </row>
     <row r="1240" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1240" s="40">
+      <c r="A1240" s="24">
         <v>45878</v>
       </c>
       <c r="B1240" s="13">
-        <v>18500.069599999999</v>
+        <v>18370.016199999998</v>
       </c>
       <c r="C1240" s="13">
-        <v>3237.6374999999998</v>
+        <v>3202.5772999999999</v>
       </c>
       <c r="D1240" s="13">
-        <v>5714.0645300778724</v>
+        <v>5736.0102439994189</v>
       </c>
       <c r="E1240" s="14">
-        <v>5189.0097614007309</v>
+        <v>5190.4546696657408</v>
       </c>
       <c r="F1240" s="13">
-        <v>691.83389999999997</v>
+        <v>690.66629999999998</v>
       </c>
       <c r="G1240" s="13">
         <v>97.894800000000004</v>
       </c>
       <c r="H1240" s="13">
-        <v>7067.1159244413393</v>
+        <v>7055.1888353620407</v>
       </c>
       <c r="I1240" s="14">
-        <v>6499.3751270625344</v>
+        <v>6497.7712544712276</v>
       </c>
       <c r="J1240" s="13">
         <v>2117.8483999999999</v>
@@ -56646,24 +56645,24 @@
       <c r="L1240" s="13"/>
       <c r="M1240" s="13"/>
       <c r="N1240" s="15">
-        <v>21309.751899999999</v>
+        <v>21178.530899999998</v>
       </c>
     </row>
     <row r="1241" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1241" s="40">
+      <c r="A1241" s="24">
         <v>45885</v>
       </c>
       <c r="B1241" s="13">
-        <v>64406.0478</v>
+        <v>64243.667600000001</v>
       </c>
       <c r="C1241" s="13">
-        <v>10978.887699999999</v>
+        <v>10935.062099999999</v>
       </c>
       <c r="D1241" s="13">
-        <v>5866.3545488310265</v>
+        <v>5875.0162561948327</v>
       </c>
       <c r="E1241" s="14">
-        <v>5324.9822287560055</v>
+        <v>5328.3289034752315</v>
       </c>
       <c r="F1241" s="13">
         <v>356.61349999999999</v>
@@ -56675,7 +56674,7 @@
         <v>4084.1946733397849</v>
       </c>
       <c r="I1241" s="14">
-        <v>6189.3239595388914</v>
+        <v>6187.5045092790242</v>
       </c>
       <c r="J1241" s="13">
         <v>12824.4524</v>
@@ -56684,25 +56683,25 @@
       <c r="L1241" s="13"/>
       <c r="M1241" s="13"/>
       <c r="N1241" s="15">
-        <v>77587.113700000002</v>
+        <v>77424.733500000002</v>
       </c>
       <c r="O1241" s="16"/>
     </row>
     <row r="1242" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1242" s="40">
+      <c r="A1242" s="24">
         <v>45892</v>
       </c>
       <c r="B1242" s="13">
-        <v>84813.881599999993</v>
+        <v>84811.044699999999</v>
       </c>
       <c r="C1242" s="13">
         <v>16082.0092</v>
       </c>
       <c r="D1242" s="13">
-        <v>5273.8361572383628</v>
+        <v>5273.6597551504947</v>
       </c>
       <c r="E1242" s="14">
-        <v>5373.2575724987</v>
+        <v>5376.1928543221784</v>
       </c>
       <c r="F1242" s="13">
         <v>1157.8651</v>
@@ -56714,33 +56713,33 @@
         <v>6080.2534679336923</v>
       </c>
       <c r="I1242" s="14">
-        <v>6195.1820338103826</v>
+        <v>6193.667101883063</v>
       </c>
       <c r="J1242" s="13">
-        <v>8321.9652999999998</v>
+        <v>8322.1689000000006</v>
       </c>
       <c r="K1242" s="13"/>
       <c r="L1242" s="13"/>
       <c r="M1242" s="13"/>
       <c r="N1242" s="15">
-        <v>94293.711999999985</v>
+        <v>94291.078699999998</v>
       </c>
     </row>
     <row r="1243" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1243" s="40">
+      <c r="A1243" s="24">
         <v>45899</v>
       </c>
       <c r="B1243" s="13">
-        <v>73311.996299999999</v>
+        <v>73084.239300000001</v>
       </c>
       <c r="C1243" s="13">
-        <v>14277.7577</v>
+        <v>14216.347299999999</v>
       </c>
       <c r="D1243" s="13">
-        <v>5134.6995684063186</v>
+        <v>5140.8591642946149</v>
       </c>
       <c r="E1243" s="14">
-        <v>5335.5276291680075</v>
+        <v>5340.0646566611076</v>
       </c>
       <c r="F1243" s="13">
         <v>913.81010000000003</v>
@@ -56752,7 +56751,7 @@
         <v>6152.8741374759629</v>
       </c>
       <c r="I1243" s="14">
-        <v>6432.0230492685823</v>
+        <v>6430.3532186571383</v>
       </c>
       <c r="J1243" s="13">
         <v>15514.602699999999</v>
@@ -56761,24 +56760,24 @@
       <c r="L1243" s="13"/>
       <c r="M1243" s="13"/>
       <c r="N1243" s="15">
-        <v>89740.409100000004</v>
+        <v>89512.652100000007</v>
       </c>
     </row>
     <row r="1244" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1244" s="40">
+      <c r="A1244" s="24">
         <v>45906</v>
       </c>
       <c r="B1244" s="13">
-        <v>48131.775500000003</v>
+        <v>47988.774299999997</v>
       </c>
       <c r="C1244" s="13">
-        <v>10071.8078</v>
+        <v>10037.602800000001</v>
       </c>
       <c r="D1244" s="13">
-        <v>4778.8615962270442</v>
+        <v>4780.8999076950913</v>
       </c>
       <c r="E1244" s="14">
-        <v>5243.1820593805478</v>
+        <v>5247.9221156296453</v>
       </c>
       <c r="F1244" s="13">
         <v>1388.6704</v>
@@ -56799,24 +56798,24 @@
       <c r="L1244" s="13"/>
       <c r="M1244" s="13"/>
       <c r="N1244" s="15">
-        <v>57701.686600000008</v>
+        <v>57558.685400000002</v>
       </c>
     </row>
     <row r="1245" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1245" s="40">
+      <c r="A1245" s="24">
         <v>45913</v>
       </c>
       <c r="B1245" s="13">
-        <v>43543.889799999997</v>
+        <v>43245.454700000002</v>
       </c>
       <c r="C1245" s="13">
-        <v>8413.2283000000007</v>
+        <v>8317.3688999999995</v>
       </c>
       <c r="D1245" s="13">
-        <v>5175.6458100631826</v>
+        <v>5199.4152501760509</v>
       </c>
       <c r="E1245" s="14">
-        <v>5060.022856253282</v>
+        <v>5065.7189729493748</v>
       </c>
       <c r="F1245" s="13">
         <v>1184.0114000000001</v>
@@ -56837,24 +56836,24 @@
       <c r="L1245" s="13"/>
       <c r="M1245" s="13"/>
       <c r="N1245" s="15">
-        <v>48936.591500000002</v>
+        <v>48638.156400000007</v>
       </c>
     </row>
     <row r="1246" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1246" s="40">
+      <c r="A1246" s="24">
         <v>45920</v>
       </c>
       <c r="B1246" s="13">
-        <v>63150.832399999999</v>
+        <v>62650.865599999997</v>
       </c>
       <c r="C1246" s="13">
-        <v>12041.887699999999</v>
+        <v>11947.379300000001</v>
       </c>
       <c r="D1246" s="13">
-        <v>5244.2635219061212</v>
+        <v>5243.900275267898</v>
       </c>
       <c r="E1246" s="14">
-        <v>5096.133011355093</v>
+        <v>5102.203082694733</v>
       </c>
       <c r="F1246" s="13">
         <v>977.74770000000001</v>
@@ -56875,24 +56874,24 @@
       <c r="L1246" s="13"/>
       <c r="M1246" s="13"/>
       <c r="N1246" s="15">
-        <v>70608.100000000006</v>
+        <v>70108.133200000011</v>
       </c>
     </row>
     <row r="1247" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1247" s="40">
+      <c r="A1247" s="24">
         <v>45927</v>
       </c>
       <c r="B1247" s="13">
-        <v>45055.311399999999</v>
+        <v>45052.244700000003</v>
       </c>
       <c r="C1247" s="13">
         <v>8526.9426000000003</v>
       </c>
       <c r="D1247" s="13">
-        <v>5283.876474083454</v>
+        <v>5283.5168258315707</v>
       </c>
       <c r="E1247" s="14">
-        <v>5098.1204413343194</v>
+        <v>5104.5708504587583</v>
       </c>
       <c r="F1247" s="13">
         <v>1625.8276000000001</v>
@@ -56913,24 +56912,24 @@
       <c r="L1247" s="13"/>
       <c r="M1247" s="13"/>
       <c r="N1247" s="15">
-        <v>60448.717899999996</v>
+        <v>60445.6512</v>
       </c>
     </row>
     <row r="1248" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A1248" s="40">
+      <c r="A1248" s="24">
         <v>45934</v>
       </c>
       <c r="B1248" s="13">
-        <v>34876.515700000004</v>
+        <v>34875.249100000001</v>
       </c>
       <c r="C1248" s="13">
         <v>7467.2049999999999</v>
       </c>
       <c r="D1248" s="13">
-        <v>4670.6251803720406</v>
+        <v>4670.4555586728902</v>
       </c>
       <c r="E1248" s="14">
-        <v>5060.9486204915502</v>
+        <v>5065.8588115488501</v>
       </c>
       <c r="F1248" s="13">
         <v>1018.4743</v>
@@ -56951,11 +56950,11 @@
       <c r="L1248" s="13"/>
       <c r="M1248" s="13"/>
       <c r="N1248" s="15">
-        <v>40655.262400000007</v>
+        <v>40653.995800000004</v>
       </c>
     </row>
     <row r="1249" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1249" s="40">
+      <c r="A1249" s="24">
         <v>45941</v>
       </c>
       <c r="B1249" s="13">
@@ -56968,7 +56967,7 @@
         <v>4382.9306781101695</v>
       </c>
       <c r="E1249" s="14">
-        <v>4974.1091561607846</v>
+        <v>4973.8861475109807</v>
       </c>
       <c r="F1249" s="13">
         <v>1116.6591000000001</v>
@@ -56993,20 +56992,20 @@
       </c>
     </row>
     <row r="1250" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1250" s="40">
+      <c r="A1250" s="24">
         <v>45948</v>
       </c>
       <c r="B1250" s="13">
-        <v>48974.020700000001</v>
+        <v>48243.912199999999</v>
       </c>
       <c r="C1250" s="13">
-        <v>9963.6882999999998</v>
+        <v>9782.5046999999995</v>
       </c>
       <c r="D1250" s="13">
-        <v>4915.2501789924527</v>
+        <v>4931.6523405299258</v>
       </c>
       <c r="E1250" s="14">
-        <v>4936.9969904882055</v>
+        <v>4941.3597020882944</v>
       </c>
       <c r="F1250" s="13">
         <v>1339.0517</v>
@@ -57027,24 +57026,24 @@
       <c r="L1250" s="13"/>
       <c r="M1250" s="13"/>
       <c r="N1250" s="15">
-        <v>62551.887300000002</v>
+        <v>61821.7788</v>
       </c>
     </row>
     <row r="1251" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1251" s="40">
+      <c r="A1251" s="24">
         <v>45955</v>
       </c>
       <c r="B1251" s="13">
-        <v>54779.7624</v>
+        <v>54509.922200000001</v>
       </c>
       <c r="C1251" s="13">
-        <v>9557.7847000000002</v>
+        <v>9494.5689999999995</v>
       </c>
       <c r="D1251" s="13">
-        <v>5731.4287901881698</v>
+        <v>5741.1686828543779</v>
       </c>
       <c r="E1251" s="14">
-        <v>5013.5433663848216</v>
+        <v>5019.6772277930168</v>
       </c>
       <c r="F1251" s="13">
         <v>1154.2166999999999</v>
@@ -57059,30 +57058,30 @@
         <v>5618.2028678006491</v>
       </c>
       <c r="J1251" s="13">
-        <v>5386.4103999999998</v>
+        <v>5375.8909000000003</v>
       </c>
       <c r="K1251" s="13"/>
       <c r="L1251" s="13"/>
       <c r="M1251" s="13"/>
       <c r="N1251" s="15">
-        <v>61320.389499999997</v>
+        <v>61040.029799999997</v>
       </c>
     </row>
     <row r="1252" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1252" s="40">
+      <c r="A1252" s="24">
         <v>45962</v>
       </c>
       <c r="B1252" s="13">
-        <v>49437.136899999998</v>
+        <v>49051.651599999997</v>
       </c>
       <c r="C1252" s="13">
-        <v>10515.293600000001</v>
+        <v>10403.208199999999</v>
       </c>
       <c r="D1252" s="13">
-        <v>4701.4509323829052</v>
+        <v>4715.0504591458621</v>
       </c>
       <c r="E1252" s="14">
-        <v>4982.2945413338712</v>
+        <v>4992.9839091483682</v>
       </c>
       <c r="F1252" s="13">
         <v>979.83450000000005</v>
@@ -57103,24 +57102,24 @@
       <c r="L1252" s="13"/>
       <c r="M1252" s="13"/>
       <c r="N1252" s="15">
-        <v>61092.325799999991</v>
+        <v>60706.840499999991</v>
       </c>
     </row>
     <row r="1253" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1253" s="40">
+      <c r="A1253" s="24">
         <v>45969</v>
       </c>
       <c r="B1253" s="13">
-        <v>88077.997900000002</v>
+        <v>88078.055699999997</v>
       </c>
       <c r="C1253" s="13">
         <v>15503.318600000001</v>
       </c>
       <c r="D1253" s="13">
-        <v>5681.2351066564552</v>
+        <v>5681.238834890486</v>
       </c>
       <c r="E1253" s="14">
-        <v>5193.2183791072102</v>
+        <v>5202.5247361039947</v>
       </c>
       <c r="F1253" s="13">
         <v>3024.5275999999999</v>
@@ -57135,17 +57134,17 @@
         <v>5539.4813027075452</v>
       </c>
       <c r="J1253" s="13">
-        <v>12275.0468</v>
+        <v>12265.096</v>
       </c>
       <c r="K1253" s="13"/>
       <c r="L1253" s="13"/>
       <c r="M1253" s="13"/>
       <c r="N1253" s="15">
-        <v>103377.5723</v>
+        <v>103367.6793</v>
       </c>
     </row>
     <row r="1254" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1254" s="40">
+      <c r="A1254" s="24">
         <v>45976</v>
       </c>
       <c r="B1254" s="13">
@@ -57158,7 +57157,7 @@
         <v>5052.8352516890982</v>
       </c>
       <c r="E1254" s="14">
-        <v>5298.1652591486372</v>
+        <v>5308.59350605891</v>
       </c>
       <c r="F1254" s="13">
         <v>2124.1673000000001</v>
@@ -57183,20 +57182,20 @@
       </c>
     </row>
     <row r="1255" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1255" s="40">
+      <c r="A1255" s="24">
         <v>45983</v>
       </c>
       <c r="B1255" s="13">
-        <v>85680.974199999997</v>
+        <v>85675.433699999994</v>
       </c>
       <c r="C1255" s="13">
         <v>13708.7893</v>
       </c>
       <c r="D1255" s="13">
-        <v>6250.0759421548628</v>
+        <v>6249.6717853851605</v>
       </c>
       <c r="E1255" s="14">
-        <v>5586.111909088565</v>
+        <v>5590.359247475978</v>
       </c>
       <c r="F1255" s="13">
         <v>2745.8622</v>
@@ -57211,30 +57210,30 @@
         <v>5979.7288428128713</v>
       </c>
       <c r="J1255" s="13">
-        <v>12449.1196</v>
+        <v>12450.415499999999</v>
       </c>
       <c r="K1255" s="13"/>
       <c r="L1255" s="13"/>
       <c r="M1255" s="13"/>
       <c r="N1255" s="15">
-        <v>100875.95600000001</v>
+        <v>100871.7114</v>
       </c>
     </row>
     <row r="1256" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1256" s="40">
+      <c r="A1256" s="24">
         <v>45990</v>
       </c>
       <c r="B1256" s="13">
-        <v>64989.205600000001</v>
+        <v>65001.712299999999</v>
       </c>
       <c r="C1256" s="13">
-        <v>12530.625599999999</v>
+        <v>12531.0414</v>
       </c>
       <c r="D1256" s="13">
-        <v>5186.4294469064662</v>
+        <v>5187.2554103923076</v>
       </c>
       <c r="E1256" s="14">
-        <v>5479.160288740447</v>
+        <v>5479.9474734858195</v>
       </c>
       <c r="F1256" s="13">
         <v>3141.94</v>
@@ -57255,11 +57254,11 @@
       <c r="L1256" s="13"/>
       <c r="M1256" s="13"/>
       <c r="N1256" s="15">
-        <v>77281.941400000011</v>
+        <v>77294.448100000009</v>
       </c>
     </row>
     <row r="1257" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1257" s="40">
+      <c r="A1257" s="24">
         <v>45997</v>
       </c>
       <c r="B1257" s="13">
@@ -57272,7 +57271,7 @@
         <v>5246.6326864924067</v>
       </c>
       <c r="E1257" s="14">
-        <v>5432.7926239141843</v>
+        <v>5432.8694834469261</v>
       </c>
       <c r="F1257" s="13">
         <v>2948.9110000000001</v>
@@ -57287,30 +57286,30 @@
         <v>6858.778759653972</v>
       </c>
       <c r="J1257" s="13">
-        <v>6890.5361999999996</v>
+        <v>6940.3462</v>
       </c>
       <c r="K1257" s="13"/>
       <c r="L1257" s="13"/>
       <c r="M1257" s="13"/>
       <c r="N1257" s="15">
-        <v>78523.970900000015</v>
+        <v>78573.780900000012</v>
       </c>
     </row>
     <row r="1258" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1258" s="40">
+      <c r="A1258" s="24">
         <v>46004</v>
       </c>
       <c r="B1258" s="13">
-        <v>60368.650399999999</v>
+        <v>60368.599000000002</v>
       </c>
       <c r="C1258" s="13">
         <v>12133.7268</v>
       </c>
       <c r="D1258" s="13">
-        <v>4975.276878658583</v>
+        <v>4975.272642532218</v>
       </c>
       <c r="E1258" s="14">
-        <v>5463.4948796555273</v>
+        <v>5463.5816890872211</v>
       </c>
       <c r="F1258" s="13">
         <v>4360.9017999999996</v>
@@ -57325,30 +57324,30 @@
         <v>7108.8683732248473</v>
       </c>
       <c r="J1258" s="13">
-        <v>10575.8716</v>
+        <v>10585.696599999999</v>
       </c>
       <c r="K1258" s="13"/>
       <c r="L1258" s="13"/>
       <c r="M1258" s="13"/>
       <c r="N1258" s="15">
-        <v>75305.42379999999</v>
+        <v>75315.197400000005</v>
       </c>
     </row>
     <row r="1259" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1259" s="40">
+      <c r="A1259" s="24">
         <v>46011</v>
       </c>
       <c r="B1259" s="13">
-        <v>65035.212</v>
+        <v>64426.640899999999</v>
       </c>
       <c r="C1259" s="13">
-        <v>11873.398800000001</v>
+        <v>11809.409900000001</v>
       </c>
       <c r="D1259" s="13">
-        <v>5477.3879910443165</v>
+        <v>5455.5343108210682</v>
       </c>
       <c r="E1259" s="14">
-        <v>5187.953227935649</v>
+        <v>5182.7833901260628</v>
       </c>
       <c r="F1259" s="13">
         <v>3014.4270000000001</v>
@@ -57363,30 +57362,30 @@
         <v>7266.6202217096234</v>
       </c>
       <c r="J1259" s="13">
-        <v>14406.8534</v>
+        <v>14233.7824</v>
       </c>
       <c r="K1259" s="13"/>
       <c r="L1259" s="13"/>
       <c r="M1259" s="13"/>
       <c r="N1259" s="15">
-        <v>82456.492399999988</v>
+        <v>81674.850299999991</v>
       </c>
     </row>
     <row r="1260" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1260" s="40">
+      <c r="A1260" s="24">
         <v>46018</v>
       </c>
       <c r="B1260" s="13">
-        <v>60703.914299999997</v>
+        <v>60702.715100000001</v>
       </c>
       <c r="C1260" s="13">
         <v>11702.9162</v>
       </c>
       <c r="D1260" s="13">
-        <v>5187.075876011143</v>
+        <v>5186.9734058251224</v>
       </c>
       <c r="E1260" s="14">
-        <v>5215.2409542684436</v>
+        <v>5209.8648911461805</v>
       </c>
       <c r="F1260" s="13">
         <v>2192.3276999999998</v>
@@ -57401,30 +57400,30 @@
         <v>6636.3073234487993</v>
       </c>
       <c r="J1260" s="13">
-        <v>7545.1985000000004</v>
+        <v>7543.9557999999997</v>
       </c>
       <c r="K1260" s="13"/>
       <c r="L1260" s="13"/>
       <c r="M1260" s="13"/>
       <c r="N1260" s="15">
-        <v>70441.440499999997</v>
+        <v>70438.998599999992</v>
       </c>
     </row>
     <row r="1261" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1261" s="40">
+      <c r="A1261" s="24">
         <v>46025</v>
       </c>
       <c r="B1261" s="13">
-        <v>36103.191599999998</v>
+        <v>36130.784399999997</v>
       </c>
       <c r="C1261" s="13">
-        <v>6765.5389999999998</v>
+        <v>6783.5308000000005</v>
       </c>
       <c r="D1261" s="13">
-        <v>5336.3363362475629</v>
+        <v>5326.2505124912232</v>
       </c>
       <c r="E1261" s="14">
-        <v>5262.9169381865267</v>
+        <v>5255.5373742530073</v>
       </c>
       <c r="F1261" s="13">
         <v>1259.8376000000001</v>
@@ -57439,89 +57438,162 @@
         <v>6388.7537797193982</v>
       </c>
       <c r="J1261" s="13">
-        <v>15486.181200000001</v>
+        <v>15412.5653</v>
       </c>
       <c r="K1261" s="13"/>
       <c r="L1261" s="13"/>
       <c r="M1261" s="13"/>
       <c r="N1261" s="15">
-        <v>52849.210399999996</v>
+        <v>52803.187299999998</v>
       </c>
     </row>
     <row r="1262" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1262" s="40">
+      <c r="A1262" s="24">
         <v>46032</v>
       </c>
       <c r="B1262" s="13">
-        <v>24362.286100000001</v>
+        <v>31640.644499999999</v>
       </c>
       <c r="C1262" s="13">
-        <v>3939.7923999999998</v>
+        <v>5683.3813</v>
       </c>
       <c r="D1262" s="13">
-        <v>6183.6471637439581</v>
+        <v>5567.2218402801864</v>
       </c>
       <c r="E1262" s="14">
-        <v>5311.6711817857731</v>
+        <v>5256.11675941047</v>
       </c>
       <c r="F1262" s="13">
-        <v>1210.1020000000001</v>
+        <v>1210.1021000000001</v>
       </c>
       <c r="G1262" s="13">
         <v>153.834</v>
       </c>
       <c r="H1262" s="13">
-        <v>7866.2844364704806</v>
+        <v>7866.2850865218361</v>
       </c>
       <c r="I1262" s="14">
-        <v>6331.7503932235877</v>
+        <v>6331.7504578958606</v>
       </c>
       <c r="J1262" s="13">
-        <v>7246.0601999999999</v>
+        <v>7770.5465000000004</v>
       </c>
       <c r="K1262" s="13"/>
       <c r="L1262" s="13"/>
       <c r="M1262" s="13"/>
       <c r="N1262" s="15">
-        <v>32818.448300000004</v>
+        <v>40621.293099999995</v>
       </c>
     </row>
     <row r="1263" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1263" s="40">
+      <c r="A1263" s="24">
         <v>46039</v>
       </c>
       <c r="B1263" s="13">
-        <v>26190.641800000001</v>
+        <v>54949.873200000002</v>
       </c>
       <c r="C1263" s="13">
-        <v>4468.2271000000001</v>
+        <v>10646.6057</v>
       </c>
       <c r="D1263" s="13">
-        <v>5861.5287929299748</v>
+        <v>5161.2574700686064</v>
       </c>
       <c r="E1263" s="14">
-        <v>5519.8142745763789</v>
+        <v>5321.8243708027785</v>
       </c>
       <c r="F1263" s="13">
-        <v>2421.2791000000002</v>
+        <v>3125.1749</v>
       </c>
       <c r="G1263" s="13">
-        <v>315.63510000000002</v>
+        <v>425.55399999999997</v>
       </c>
       <c r="H1263" s="13">
-        <v>7671.1338504494588</v>
+        <v>7343.7798728246007</v>
       </c>
       <c r="I1263" s="14">
-        <v>6149.912181129077</v>
+        <v>6168.4749481004819</v>
       </c>
       <c r="J1263" s="13">
-        <v>3253.4405000000002</v>
+        <v>7663.2416999999996</v>
       </c>
       <c r="K1263" s="13"/>
       <c r="L1263" s="13"/>
       <c r="M1263" s="13"/>
       <c r="N1263" s="15">
-        <v>31865.361400000002</v>
+        <v>65738.289799999999</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A1264" s="24">
+        <v>46046</v>
+      </c>
+      <c r="B1264" s="13">
+        <v>36861.675300000003</v>
+      </c>
+      <c r="C1264" s="13">
+        <v>6583.4578000000001</v>
+      </c>
+      <c r="D1264" s="13">
+        <v>5599.1359586143326</v>
+      </c>
+      <c r="E1264" s="14">
+        <v>5371.2274254038402</v>
+      </c>
+      <c r="F1264" s="13">
+        <v>2057.6224999999999</v>
+      </c>
+      <c r="G1264" s="13">
+        <v>305.68990000000002</v>
+      </c>
+      <c r="H1264" s="13">
+        <v>6731.0778013928493</v>
+      </c>
+      <c r="I1264" s="14">
+        <v>6574.3544445201833</v>
+      </c>
+      <c r="J1264" s="13">
+        <v>5694.7548999999999</v>
+      </c>
+      <c r="K1264" s="13"/>
+      <c r="L1264" s="13"/>
+      <c r="M1264" s="13"/>
+      <c r="N1264" s="15">
+        <v>44614.0527</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A1265" s="20">
+        <v>46053</v>
+      </c>
+      <c r="B1265" s="22">
+        <v>39309.172100000003</v>
+      </c>
+      <c r="C1265" s="22">
+        <v>6946.4452000000001</v>
+      </c>
+      <c r="D1265" s="22">
+        <v>5658.8904062757165</v>
+      </c>
+      <c r="E1265" s="23">
+        <v>5394.1002568499107</v>
+      </c>
+      <c r="F1265" s="22">
+        <v>957.96249999999998</v>
+      </c>
+      <c r="G1265" s="22">
+        <v>146.49180000000001</v>
+      </c>
+      <c r="H1265" s="22">
+        <v>6539.3591996275554</v>
+      </c>
+      <c r="I1265" s="23">
+        <v>7081.0976445614751</v>
+      </c>
+      <c r="J1265" s="22">
+        <v>5487.8076000000001</v>
+      </c>
+      <c r="N1265" s="21">
+        <v>45754.942200000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion: backend (MacroData, Licitaciones LRM PDF, cotizaciones, inflacion implicita), scripts update (027 tipo cambio columna CIERRE BCU BILLETE, _helpers sys.path, tpm_uyu download), datos historicos y direct/calculate
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/data_raw/serie_semanal_ingreso_medio_exportacion_inac.xlsx
+++ b/data_raw/serie_semanal_ingreso_medio_exportacion_inac.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\inac.local\archivos\GIF\Datos y Estadísticas\Publicaciones Web\Públicos\Boletín Semanal\Salidas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6B11AD-E333-4194-925B-E30830FBE961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DCB66C-274A-498A-BC70-D06BED4FCFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -807,13 +807,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W1265"/>
+  <dimension ref="A1:W1266"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B1258" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B1261" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F1270" sqref="F1270"/>
+      <selection pane="bottomRight" activeCell="C1273" sqref="C1273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -923,8 +923,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="35">
-        <f ca="1">TODAY()</f>
-        <v>46057</v>
+        <v>46064</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -53546,7 +53545,7 @@
         <v>3757.2628855111907</v>
       </c>
       <c r="E1159" s="14">
-        <v>3780.2897920809946</v>
+        <v>3780.289792080996</v>
       </c>
       <c r="F1159" s="13">
         <v>1494.2402999999999</v>
@@ -53584,7 +53583,7 @@
         <v>3966.9774403598576</v>
       </c>
       <c r="E1160" s="14">
-        <v>3927.1454924749787</v>
+        <v>3927.1454924749778</v>
       </c>
       <c r="F1160" s="13">
         <v>1675.7801999999999</v>
@@ -53622,7 +53621,7 @@
         <v>3836.9166844383958</v>
       </c>
       <c r="E1161" s="14">
-        <v>3873.8651916427139</v>
+        <v>3873.8651916427129</v>
       </c>
       <c r="F1161" s="13">
         <v>1355.5396000000001</v>
@@ -53748,7 +53747,7 @@
         <v>3294.3855571640811</v>
       </c>
       <c r="I1164" s="14">
-        <v>3579.4806019611092</v>
+        <v>3579.4806019611101</v>
       </c>
       <c r="J1164" s="13">
         <v>14285.5708</v>
@@ -53774,7 +53773,7 @@
         <v>4422.3044460821966</v>
       </c>
       <c r="E1165" s="14">
-        <v>4180.3219217309888</v>
+        <v>4180.3219217309879</v>
       </c>
       <c r="F1165" s="13">
         <v>1064.4956999999999</v>
@@ -53786,7 +53785,7 @@
         <v>3930.3634262421583</v>
       </c>
       <c r="I1165" s="14">
-        <v>3575.1060841405902</v>
+        <v>3575.1060841405915</v>
       </c>
       <c r="J1165" s="13">
         <v>4062.5365999999999</v>
@@ -53862,7 +53861,7 @@
         <v>3239.1375010965894</v>
       </c>
       <c r="I1167" s="14">
-        <v>3596.9869038721486</v>
+        <v>3596.986903872149</v>
       </c>
       <c r="J1167" s="13">
         <v>7280.7353999999996</v>
@@ -54154,7 +54153,7 @@
         <v>4151.5723390857438</v>
       </c>
       <c r="E1175" s="14">
-        <v>3955.4372729635284</v>
+        <v>3955.4372729635274</v>
       </c>
       <c r="F1175" s="13">
         <v>1393.8427999999999</v>
@@ -54166,7 +54165,7 @@
         <v>3165.986834005897</v>
       </c>
       <c r="I1175" s="14">
-        <v>3345.9193035632725</v>
+        <v>3345.9193035632734</v>
       </c>
       <c r="J1175" s="13">
         <v>18463.542600000001</v>
@@ -54230,7 +54229,7 @@
         <v>4611.2745069454377</v>
       </c>
       <c r="E1177" s="14">
-        <v>4199.3537107264337</v>
+        <v>4199.3537107264319</v>
       </c>
       <c r="F1177" s="13">
         <v>850.38009999999997</v>
@@ -54306,7 +54305,7 @@
         <v>4256.7265580616331</v>
       </c>
       <c r="E1179" s="14">
-        <v>4295.134471414779</v>
+        <v>4295.1344714147781</v>
       </c>
       <c r="F1179" s="13">
         <v>1120.1349</v>
@@ -54344,7 +54343,7 @@
         <v>4008.5523747206912</v>
       </c>
       <c r="E1180" s="14">
-        <v>4173.750113280712</v>
+        <v>4173.750113280711</v>
       </c>
       <c r="F1180" s="13">
         <v>909.47910000000002</v>
@@ -54534,7 +54533,7 @@
         <v>4059.2289950562249</v>
       </c>
       <c r="E1185" s="14">
-        <v>4136.2469995879537</v>
+        <v>4136.2469995879528</v>
       </c>
       <c r="F1185" s="13">
         <v>566.73659999999995</v>
@@ -54546,7 +54545,7 @@
         <v>4503.2383558639631</v>
       </c>
       <c r="I1185" s="14">
-        <v>4446.3732870828389</v>
+        <v>4446.3732870828371</v>
       </c>
       <c r="J1185" s="13">
         <v>3367.5416</v>
@@ -54800,7 +54799,7 @@
         <v>3714.6529959308918</v>
       </c>
       <c r="E1192" s="14">
-        <v>4249.8371965672713</v>
+        <v>4249.8371965672723</v>
       </c>
       <c r="F1192" s="13">
         <v>915.8922</v>
@@ -54838,7 +54837,7 @@
         <v>4559.5761948121963</v>
       </c>
       <c r="E1193" s="14">
-        <v>4357.0783156354555</v>
+        <v>4357.0783156354564</v>
       </c>
       <c r="F1193" s="13">
         <v>1482.4329</v>
@@ -54876,7 +54875,7 @@
         <v>4046.3203203871026</v>
       </c>
       <c r="E1194" s="14">
-        <v>4089.7449537136222</v>
+        <v>4089.744953713624</v>
       </c>
       <c r="F1194" s="13">
         <v>545.97190000000001</v>
@@ -55066,7 +55065,7 @@
         <v>4811.1216968574927</v>
       </c>
       <c r="E1199" s="14">
-        <v>4410.8853143259776</v>
+        <v>4410.8853143259794</v>
       </c>
       <c r="F1199" s="13">
         <v>923.27440000000001</v>
@@ -55142,7 +55141,7 @@
         <v>4458.3467251750426</v>
       </c>
       <c r="E1201" s="14">
-        <v>4487.7143253551785</v>
+        <v>4487.7143253551803</v>
       </c>
       <c r="F1201" s="13">
         <v>1677.1370999999999</v>
@@ -55370,7 +55369,7 @@
         <v>4252.7279635792374</v>
       </c>
       <c r="E1207" s="14">
-        <v>4389.4044684956043</v>
+        <v>4389.4044684956052</v>
       </c>
       <c r="F1207" s="13">
         <v>1109.1464000000001</v>
@@ -55382,7 +55381,7 @@
         <v>4145.9867547787508</v>
       </c>
       <c r="I1207" s="14">
-        <v>4315.8033455629666</v>
+        <v>4315.8033455629657</v>
       </c>
       <c r="J1207" s="13">
         <v>8213.6905999999999</v>
@@ -55420,7 +55419,7 @@
         <v>4947.3851972485918</v>
       </c>
       <c r="I1208" s="14">
-        <v>4350.8974691132007</v>
+        <v>4350.8974691131998</v>
       </c>
       <c r="J1208" s="13">
         <v>9287.4572000000007</v>
@@ -55475,16 +55474,16 @@
         <v>45668</v>
       </c>
       <c r="B1210" s="13">
-        <v>39758.819600000003</v>
+        <v>39757.1345</v>
       </c>
       <c r="C1210" s="13">
         <v>8771.9485000000004</v>
       </c>
       <c r="D1210" s="13">
-        <v>4532.4957847164742</v>
+        <v>4532.3036837254567</v>
       </c>
       <c r="E1210" s="14">
-        <v>4508.6319604314422</v>
+        <v>4508.5895396139722</v>
       </c>
       <c r="F1210" s="13">
         <v>1813.4111</v>
@@ -55496,7 +55495,7 @@
         <v>6882.5719118850975</v>
       </c>
       <c r="I1210" s="14">
-        <v>5131.0721532756543</v>
+        <v>5131.0721532756534</v>
       </c>
       <c r="J1210" s="13">
         <v>5833.4898999999996</v>
@@ -55505,7 +55504,7 @@
       <c r="L1210" s="13"/>
       <c r="M1210" s="13"/>
       <c r="N1210" s="15">
-        <v>47405.720600000001</v>
+        <v>47404.035499999998</v>
       </c>
     </row>
     <row r="1211" spans="1:14" ht="15.75" customHeight="1">
@@ -55522,7 +55521,7 @@
         <v>4637.0540275804779</v>
       </c>
       <c r="E1211" s="14">
-        <v>4537.1133140358179</v>
+        <v>4537.0690492475896</v>
       </c>
       <c r="F1211" s="13">
         <v>1790.9604999999999</v>
@@ -55534,7 +55533,7 @@
         <v>6099.4532507976128</v>
       </c>
       <c r="I1211" s="14">
-        <v>5615.5313175907386</v>
+        <v>5615.5313175907377</v>
       </c>
       <c r="J1211" s="13">
         <v>4923.6122999999998</v>
@@ -55560,7 +55559,7 @@
         <v>4833.6383582173466</v>
       </c>
       <c r="E1212" s="14">
-        <v>4670.5434936426145</v>
+        <v>4670.4968488940985</v>
       </c>
       <c r="F1212" s="13">
         <v>1637.0943</v>
@@ -55598,7 +55597,7 @@
         <v>4746.7946040659472</v>
       </c>
       <c r="E1213" s="14">
-        <v>4691.500419453695</v>
+        <v>4691.4576149978011</v>
       </c>
       <c r="F1213" s="13">
         <v>2092.5389</v>
@@ -55648,7 +55647,7 @@
         <v>5483.9420094229508</v>
       </c>
       <c r="I1214" s="14">
-        <v>5618.8491234155326</v>
+        <v>5618.8491234155317</v>
       </c>
       <c r="J1214" s="13">
         <v>8807.2849999999999</v>
@@ -55724,7 +55723,7 @@
         <v>4337.7130954170489</v>
       </c>
       <c r="I1216" s="14">
-        <v>4764.4312599888563</v>
+        <v>4764.4312599888553</v>
       </c>
       <c r="J1216" s="13">
         <v>3920.1588999999999</v>
@@ -55826,7 +55825,7 @@
         <v>4760.4158560393298</v>
       </c>
       <c r="E1219" s="14">
-        <v>4756.3449304404703</v>
+        <v>4756.3449304404712</v>
       </c>
       <c r="F1219" s="13">
         <v>1866.9058</v>
@@ -55902,7 +55901,7 @@
         <v>4701.8076037281035</v>
       </c>
       <c r="E1221" s="14">
-        <v>4670.547347196818</v>
+        <v>4670.5473471968171</v>
       </c>
       <c r="F1221" s="13">
         <v>673.16070000000002</v>
@@ -55940,7 +55939,7 @@
         <v>4851.1377242434155</v>
       </c>
       <c r="E1222" s="14">
-        <v>4695.9889906735043</v>
+        <v>4695.9889906735052</v>
       </c>
       <c r="F1222" s="13">
         <v>1081.6878999999999</v>
@@ -55978,7 +55977,7 @@
         <v>4613.3343787360272</v>
       </c>
       <c r="E1223" s="14">
-        <v>4695.6528467809921</v>
+        <v>4695.6528467809931</v>
       </c>
       <c r="F1223" s="13">
         <v>1661.2738999999999</v>
@@ -56168,7 +56167,7 @@
         <v>5174.2919588572313</v>
       </c>
       <c r="E1228" s="14">
-        <v>5048.416067317241</v>
+        <v>5048.41606731724</v>
       </c>
       <c r="F1228" s="13">
         <v>677.62339999999995</v>
@@ -56206,7 +56205,7 @@
         <v>5128.5357907447842</v>
       </c>
       <c r="E1229" s="14">
-        <v>4984.0678413824007</v>
+        <v>4984.0678413823998</v>
       </c>
       <c r="F1229" s="13">
         <v>465.10070000000002</v>
@@ -56273,16 +56272,16 @@
         <v>45815</v>
       </c>
       <c r="B1231" s="13">
-        <v>59293.639499999997</v>
+        <v>59293.162300000004</v>
       </c>
       <c r="C1231" s="13">
         <v>12502.961600000001</v>
       </c>
       <c r="D1231" s="13">
-        <v>4742.3675603386637</v>
+        <v>4742.3293933814848</v>
       </c>
       <c r="E1231" s="14">
-        <v>4961.7219908251109</v>
+        <v>4961.7135906734002</v>
       </c>
       <c r="F1231" s="13">
         <v>1023.9116</v>
@@ -56303,7 +56302,7 @@
       <c r="L1231" s="13"/>
       <c r="M1231" s="13"/>
       <c r="N1231" s="15">
-        <v>75299.767500000002</v>
+        <v>75299.290300000008</v>
       </c>
     </row>
     <row r="1232" spans="1:14" ht="15.75" customHeight="1">
@@ -56320,7 +56319,7 @@
         <v>4822.1163386837061</v>
       </c>
       <c r="E1232" s="14">
-        <v>4910.1042400789902</v>
+        <v>4910.0949138408505</v>
       </c>
       <c r="F1232" s="13">
         <v>1933.1436000000001</v>
@@ -56349,16 +56348,16 @@
         <v>45829</v>
       </c>
       <c r="B1233" s="13">
-        <v>46291.854700000004</v>
+        <v>46290.895499999999</v>
       </c>
       <c r="C1233" s="13">
         <v>9420.8922999999995</v>
       </c>
       <c r="D1233" s="13">
-        <v>4913.7441789882268</v>
+        <v>4913.6423627303329</v>
       </c>
       <c r="E1233" s="14">
-        <v>4836.469487737555</v>
+        <v>4836.4394194233882</v>
       </c>
       <c r="F1233" s="13">
         <v>910.61059999999998</v>
@@ -56379,7 +56378,7 @@
       <c r="L1233" s="13"/>
       <c r="M1233" s="13"/>
       <c r="N1233" s="15">
-        <v>54101.474500000004</v>
+        <v>54100.515299999999</v>
       </c>
     </row>
     <row r="1234" spans="1:15" ht="15.75" customHeight="1">
@@ -56396,7 +56395,7 @@
         <v>4900.5613652109014</v>
       </c>
       <c r="E1234" s="14">
-        <v>4766.381961573491</v>
+        <v>4766.3500544760827</v>
       </c>
       <c r="F1234" s="13">
         <v>556.48080000000004</v>
@@ -56408,7 +56407,7 @@
         <v>6232.9559455378785</v>
       </c>
       <c r="I1234" s="14">
-        <v>6273.3822151253535</v>
+        <v>6273.3822151253544</v>
       </c>
       <c r="J1234" s="13">
         <v>8405.0920000000006</v>
@@ -56434,7 +56433,7 @@
         <v>5125.621659266998</v>
       </c>
       <c r="E1235" s="14">
-        <v>4955.4276592396536</v>
+        <v>4955.3969607385388</v>
       </c>
       <c r="F1235" s="13">
         <v>1182.9712999999999</v>
@@ -56446,7 +56445,7 @@
         <v>5270.8131997196551</v>
       </c>
       <c r="I1235" s="14">
-        <v>6279.4686229430445</v>
+        <v>6279.4686229430436</v>
       </c>
       <c r="J1235" s="13">
         <v>12601.2554</v>
@@ -56463,16 +56462,16 @@
         <v>45850</v>
       </c>
       <c r="B1236" s="13">
-        <v>38590.557000000001</v>
+        <v>38585.658499999998</v>
       </c>
       <c r="C1236" s="13">
         <v>8635.1026999999995</v>
       </c>
       <c r="D1236" s="13">
-        <v>4469.0327771087195</v>
+        <v>4468.4654995475621</v>
       </c>
       <c r="E1236" s="14">
-        <v>4833.627777242179</v>
+        <v>4833.5005717752974</v>
       </c>
       <c r="F1236" s="13">
         <v>509.77510000000001</v>
@@ -56493,7 +56492,7 @@
       <c r="L1236" s="13"/>
       <c r="M1236" s="13"/>
       <c r="N1236" s="15">
-        <v>46134.5409</v>
+        <v>46129.642399999997</v>
       </c>
     </row>
     <row r="1237" spans="1:15" ht="15.75" customHeight="1">
@@ -56510,7 +56509,7 @@
         <v>5279.8066063917322</v>
       </c>
       <c r="E1237" s="14">
-        <v>4927.3911159242625</v>
+        <v>4927.2749374102932</v>
       </c>
       <c r="F1237" s="13">
         <v>770.73030000000006</v>
@@ -56548,7 +56547,7 @@
         <v>5523.9290394646114</v>
       </c>
       <c r="E1238" s="14">
-        <v>5022.0176430942774</v>
+        <v>5021.9091692425382</v>
       </c>
       <c r="F1238" s="13">
         <v>937.15679999999998</v>
@@ -56560,7 +56559,7 @@
         <v>5904.8972833195967</v>
       </c>
       <c r="I1238" s="14">
-        <v>5662.7424793253513</v>
+        <v>5662.7424793253522</v>
       </c>
       <c r="J1238" s="13">
         <v>5018.8672999999999</v>
@@ -56577,16 +56576,16 @@
         <v>45871</v>
       </c>
       <c r="B1239" s="13">
-        <v>54997.7889</v>
+        <v>54996.925199999998</v>
       </c>
       <c r="C1239" s="13">
         <v>10955.508</v>
       </c>
       <c r="D1239" s="13">
-        <v>5020.1039422361791</v>
+        <v>5020.0251051799696</v>
       </c>
       <c r="E1239" s="14">
-        <v>4984.0247080089212</v>
+        <v>4983.8947731923981</v>
       </c>
       <c r="F1239" s="13">
         <v>1951.8497</v>
@@ -56598,7 +56597,7 @@
         <v>6823.3180379492396</v>
       </c>
       <c r="I1239" s="14">
-        <v>6067.7529720316088</v>
+        <v>6067.7529720316097</v>
       </c>
       <c r="J1239" s="13">
         <v>8211.3163000000004</v>
@@ -56607,7 +56606,7 @@
       <c r="L1239" s="13"/>
       <c r="M1239" s="13"/>
       <c r="N1239" s="15">
-        <v>65160.954899999997</v>
+        <v>65160.091199999995</v>
       </c>
     </row>
     <row r="1240" spans="1:15" ht="15.75" customHeight="1">
@@ -56624,7 +56623,7 @@
         <v>5736.0102439994189</v>
       </c>
       <c r="E1240" s="14">
-        <v>5190.4546696657408</v>
+        <v>5190.3317916635515</v>
       </c>
       <c r="F1240" s="13">
         <v>690.66629999999998</v>
@@ -56636,7 +56635,7 @@
         <v>7055.1888353620407</v>
       </c>
       <c r="I1240" s="14">
-        <v>6497.7712544712276</v>
+        <v>6497.7712544712294</v>
       </c>
       <c r="J1240" s="13">
         <v>2117.8483999999999</v>
@@ -56662,7 +56661,7 @@
         <v>5875.0162561948327</v>
       </c>
       <c r="E1241" s="14">
-        <v>5328.3289034752315</v>
+        <v>5328.3062561328534</v>
       </c>
       <c r="F1241" s="13">
         <v>356.61349999999999</v>
@@ -56692,16 +56691,16 @@
         <v>45892</v>
       </c>
       <c r="B1242" s="13">
-        <v>84811.044699999999</v>
+        <v>84756.180800000002</v>
       </c>
       <c r="C1242" s="13">
         <v>16082.0092</v>
       </c>
       <c r="D1242" s="13">
-        <v>5273.6597551504947</v>
+        <v>5270.2482473396421</v>
       </c>
       <c r="E1242" s="14">
-        <v>5376.1928543221784</v>
+        <v>5374.9209094320613</v>
       </c>
       <c r="F1242" s="13">
         <v>1157.8651</v>
@@ -56713,7 +56712,7 @@
         <v>6080.2534679336923</v>
       </c>
       <c r="I1242" s="14">
-        <v>6193.667101883063</v>
+        <v>6193.6671018830639</v>
       </c>
       <c r="J1242" s="13">
         <v>8322.1689000000006</v>
@@ -56722,7 +56721,7 @@
       <c r="L1242" s="13"/>
       <c r="M1242" s="13"/>
       <c r="N1242" s="15">
-        <v>94291.078699999998</v>
+        <v>94236.214800000002</v>
       </c>
     </row>
     <row r="1243" spans="1:15" ht="15.75" customHeight="1">
@@ -56730,16 +56729,16 @@
         <v>45899</v>
       </c>
       <c r="B1243" s="13">
-        <v>73084.239300000001</v>
+        <v>73082.8802</v>
       </c>
       <c r="C1243" s="13">
         <v>14216.347299999999</v>
       </c>
       <c r="D1243" s="13">
-        <v>5140.8591642946149</v>
+        <v>5140.7635630848727</v>
       </c>
       <c r="E1243" s="14">
-        <v>5340.0646566611076</v>
+        <v>5338.9335921856164</v>
       </c>
       <c r="F1243" s="13">
         <v>913.81010000000003</v>
@@ -56760,7 +56759,7 @@
       <c r="L1243" s="13"/>
       <c r="M1243" s="13"/>
       <c r="N1243" s="15">
-        <v>89512.652100000007</v>
+        <v>89511.293000000005</v>
       </c>
     </row>
     <row r="1244" spans="1:15" ht="15.75" customHeight="1">
@@ -56777,7 +56776,7 @@
         <v>4780.8999076950913</v>
       </c>
       <c r="E1244" s="14">
-        <v>5247.9221156296453</v>
+        <v>5246.8519676962314</v>
       </c>
       <c r="F1244" s="13">
         <v>1388.6704</v>
@@ -56815,7 +56814,7 @@
         <v>5199.4152501760509</v>
       </c>
       <c r="E1245" s="14">
-        <v>5065.7189729493748</v>
+        <v>5064.6400874631245</v>
       </c>
       <c r="F1245" s="13">
         <v>1184.0114000000001</v>
@@ -56853,7 +56852,7 @@
         <v>5243.900275267898</v>
       </c>
       <c r="E1246" s="14">
-        <v>5102.203082694733</v>
+        <v>5102.1744621158523</v>
       </c>
       <c r="F1246" s="13">
         <v>977.74770000000001</v>
@@ -56929,7 +56928,7 @@
         <v>4670.4555586728902</v>
       </c>
       <c r="E1248" s="14">
-        <v>5065.8588115488501</v>
+        <v>5065.8588115488492</v>
       </c>
       <c r="F1248" s="13">
         <v>1018.4743</v>
@@ -57017,7 +57016,7 @@
         <v>6096.8579855739072</v>
       </c>
       <c r="I1250" s="14">
-        <v>5726.2108069747692</v>
+        <v>5726.2108069747683</v>
       </c>
       <c r="J1250" s="13">
         <v>12238.814899999999</v>
@@ -57055,7 +57054,7 @@
         <v>4751.1729571527949</v>
       </c>
       <c r="I1251" s="14">
-        <v>5618.2028678006491</v>
+        <v>5618.20286780065</v>
       </c>
       <c r="J1251" s="13">
         <v>5375.8909000000003</v>
@@ -57072,16 +57071,16 @@
         <v>45962</v>
       </c>
       <c r="B1252" s="13">
-        <v>49051.651599999997</v>
+        <v>49051.051599999999</v>
       </c>
       <c r="C1252" s="13">
         <v>10403.208199999999</v>
       </c>
       <c r="D1252" s="13">
-        <v>4715.0504591458621</v>
+        <v>4714.9927846296496</v>
       </c>
       <c r="E1252" s="14">
-        <v>4992.9839091483682</v>
+        <v>4992.9674924973551</v>
       </c>
       <c r="F1252" s="13">
         <v>979.83450000000005</v>
@@ -57102,7 +57101,7 @@
       <c r="L1252" s="13"/>
       <c r="M1252" s="13"/>
       <c r="N1252" s="15">
-        <v>60706.840499999991</v>
+        <v>60706.2405</v>
       </c>
     </row>
     <row r="1253" spans="1:14" ht="15.75" customHeight="1">
@@ -57113,13 +57112,13 @@
         <v>88078.055699999997</v>
       </c>
       <c r="C1253" s="13">
-        <v>15503.318600000001</v>
+        <v>15503.728800000001</v>
       </c>
       <c r="D1253" s="13">
-        <v>5681.238834890486</v>
+        <v>5681.0885198146652</v>
       </c>
       <c r="E1253" s="14">
-        <v>5202.5247361039947</v>
+        <v>5202.4701264931327</v>
       </c>
       <c r="F1253" s="13">
         <v>3024.5275999999999</v>
@@ -57148,16 +57147,16 @@
         <v>45976</v>
       </c>
       <c r="B1254" s="13">
-        <v>45134.0219</v>
+        <v>45133.856899999999</v>
       </c>
       <c r="C1254" s="13">
         <v>8932.4151000000002</v>
       </c>
       <c r="D1254" s="13">
-        <v>5052.8352516890982</v>
+        <v>5052.8167796411517</v>
       </c>
       <c r="E1254" s="14">
-        <v>5308.59350605891</v>
+        <v>5308.5292769043917</v>
       </c>
       <c r="F1254" s="13">
         <v>2124.1673000000001</v>
@@ -57178,7 +57177,7 @@
       <c r="L1254" s="13"/>
       <c r="M1254" s="13"/>
       <c r="N1254" s="15">
-        <v>57832.553200000002</v>
+        <v>57832.388200000001</v>
       </c>
     </row>
     <row r="1255" spans="1:14" ht="15.75" customHeight="1">
@@ -57186,16 +57185,16 @@
         <v>45983</v>
       </c>
       <c r="B1255" s="13">
-        <v>85675.433699999994</v>
+        <v>84503.003200000006</v>
       </c>
       <c r="C1255" s="13">
-        <v>13708.7893</v>
+        <v>13591.8501</v>
       </c>
       <c r="D1255" s="13">
-        <v>6249.6717853851605</v>
+        <v>6217.1818095610106</v>
       </c>
       <c r="E1255" s="14">
-        <v>5590.359247475978</v>
+        <v>5580.876229429512</v>
       </c>
       <c r="F1255" s="13">
         <v>2745.8622</v>
@@ -57216,7 +57215,7 @@
       <c r="L1255" s="13"/>
       <c r="M1255" s="13"/>
       <c r="N1255" s="15">
-        <v>100871.7114</v>
+        <v>99699.280900000012</v>
       </c>
     </row>
     <row r="1256" spans="1:14" ht="15.75" customHeight="1">
@@ -57233,7 +57232,7 @@
         <v>5187.2554103923076</v>
       </c>
       <c r="E1256" s="14">
-        <v>5479.9474734858195</v>
+        <v>5470.8196209791013</v>
       </c>
       <c r="F1256" s="13">
         <v>3141.94</v>
@@ -57262,16 +57261,16 @@
         <v>45997</v>
       </c>
       <c r="B1257" s="13">
-        <v>68684.523700000005</v>
+        <v>68682.279200000004</v>
       </c>
       <c r="C1257" s="13">
         <v>13091.163</v>
       </c>
       <c r="D1257" s="13">
-        <v>5246.6326864924067</v>
+        <v>5246.4612349567415</v>
       </c>
       <c r="E1257" s="14">
-        <v>5432.8694834469261</v>
+        <v>5422.8728491686034</v>
       </c>
       <c r="F1257" s="13">
         <v>2948.9110000000001</v>
@@ -57292,7 +57291,7 @@
       <c r="L1257" s="13"/>
       <c r="M1257" s="13"/>
       <c r="N1257" s="15">
-        <v>78573.780900000012</v>
+        <v>78571.536400000012</v>
       </c>
     </row>
     <row r="1258" spans="1:14" ht="15.75" customHeight="1">
@@ -57309,7 +57308,7 @@
         <v>4975.272642532218</v>
       </c>
       <c r="E1258" s="14">
-        <v>5463.5816890872211</v>
+        <v>5453.542739051486</v>
       </c>
       <c r="F1258" s="13">
         <v>4360.9017999999996</v>
@@ -57338,16 +57337,16 @@
         <v>46011</v>
       </c>
       <c r="B1259" s="13">
-        <v>64426.640899999999</v>
+        <v>64423.140599999999</v>
       </c>
       <c r="C1259" s="13">
         <v>11809.409900000001</v>
       </c>
       <c r="D1259" s="13">
-        <v>5455.5343108210682</v>
+        <v>5455.2379115911626</v>
       </c>
       <c r="E1259" s="14">
-        <v>5182.7833901260628</v>
+        <v>5182.6739864638521</v>
       </c>
       <c r="F1259" s="13">
         <v>3014.4270000000001</v>
@@ -57368,7 +57367,7 @@
       <c r="L1259" s="13"/>
       <c r="M1259" s="13"/>
       <c r="N1259" s="15">
-        <v>81674.850299999991</v>
+        <v>81671.349999999991</v>
       </c>
     </row>
     <row r="1260" spans="1:14" ht="15.75" customHeight="1">
@@ -57376,16 +57375,16 @@
         <v>46018</v>
       </c>
       <c r="B1260" s="13">
-        <v>60702.715100000001</v>
+        <v>60699.285100000001</v>
       </c>
       <c r="C1260" s="13">
         <v>11702.9162</v>
       </c>
       <c r="D1260" s="13">
-        <v>5186.9734058251224</v>
+        <v>5186.680316483852</v>
       </c>
       <c r="E1260" s="14">
-        <v>5209.8648911461805</v>
+        <v>5209.6862472592102</v>
       </c>
       <c r="F1260" s="13">
         <v>2192.3276999999998</v>
@@ -57406,7 +57405,7 @@
       <c r="L1260" s="13"/>
       <c r="M1260" s="13"/>
       <c r="N1260" s="15">
-        <v>70438.998599999992</v>
+        <v>70435.568599999999</v>
       </c>
     </row>
     <row r="1261" spans="1:14" ht="15.75" customHeight="1">
@@ -57414,16 +57413,16 @@
         <v>46025</v>
       </c>
       <c r="B1261" s="13">
-        <v>36130.784399999997</v>
+        <v>36129.719400000002</v>
       </c>
       <c r="C1261" s="13">
         <v>6783.5308000000005</v>
       </c>
       <c r="D1261" s="13">
-        <v>5326.2505124912232</v>
+        <v>5326.0935146045176</v>
       </c>
       <c r="E1261" s="14">
-        <v>5255.5373742530073</v>
+        <v>5255.3639159833792</v>
       </c>
       <c r="F1261" s="13">
         <v>1259.8376000000001</v>
@@ -57444,7 +57443,7 @@
       <c r="L1261" s="13"/>
       <c r="M1261" s="13"/>
       <c r="N1261" s="15">
-        <v>52803.187299999998</v>
+        <v>52802.122300000003</v>
       </c>
     </row>
     <row r="1262" spans="1:14" ht="15.75" customHeight="1">
@@ -57461,7 +57460,7 @@
         <v>5567.2218402801864</v>
       </c>
       <c r="E1262" s="14">
-        <v>5256.11675941047</v>
+        <v>5255.9253788488613</v>
       </c>
       <c r="F1262" s="13">
         <v>1210.1021000000001</v>
@@ -57490,37 +57489,37 @@
         <v>46039</v>
       </c>
       <c r="B1263" s="13">
-        <v>54949.873200000002</v>
+        <v>58966.716099999998</v>
       </c>
       <c r="C1263" s="13">
-        <v>10646.6057</v>
+        <v>11294.476500000001</v>
       </c>
       <c r="D1263" s="13">
-        <v>5161.2574700686064</v>
+        <v>5220.845437147972</v>
       </c>
       <c r="E1263" s="14">
-        <v>5321.8243708027785</v>
+        <v>5335.3901554128042</v>
       </c>
       <c r="F1263" s="13">
-        <v>3125.1749</v>
+        <v>3212.6219999999998</v>
       </c>
       <c r="G1263" s="13">
-        <v>425.55399999999997</v>
+        <v>433.1001</v>
       </c>
       <c r="H1263" s="13">
-        <v>7343.7798728246007</v>
+        <v>7417.7355304235671</v>
       </c>
       <c r="I1263" s="14">
-        <v>6168.4749481004819</v>
+        <v>6195.5463753536742</v>
       </c>
       <c r="J1263" s="13">
-        <v>7663.2416999999996</v>
+        <v>7824.2637999999997</v>
       </c>
       <c r="K1263" s="13"/>
       <c r="L1263" s="13"/>
       <c r="M1263" s="13"/>
       <c r="N1263" s="15">
-        <v>65738.289799999999</v>
+        <v>70003.601899999994</v>
       </c>
     </row>
     <row r="1264" spans="1:14" ht="15.75" customHeight="1">
@@ -57528,37 +57527,37 @@
         <v>46046</v>
       </c>
       <c r="B1264" s="13">
-        <v>36861.675300000003</v>
+        <v>40276.888800000001</v>
       </c>
       <c r="C1264" s="13">
-        <v>6583.4578000000001</v>
+        <v>7173.5888000000004</v>
       </c>
       <c r="D1264" s="13">
-        <v>5599.1359586143326</v>
+        <v>5614.6079630323939</v>
       </c>
       <c r="E1264" s="14">
-        <v>5371.2274254038402</v>
+        <v>5393.7805058135591</v>
       </c>
       <c r="F1264" s="13">
-        <v>2057.6224999999999</v>
+        <v>2043.3688</v>
       </c>
       <c r="G1264" s="13">
         <v>305.68990000000002</v>
       </c>
       <c r="H1264" s="13">
-        <v>6731.0778013928493</v>
+        <v>6684.4498297130522</v>
       </c>
       <c r="I1264" s="14">
-        <v>6574.3544445201833</v>
+        <v>6593.7417610129596</v>
       </c>
       <c r="J1264" s="13">
-        <v>5694.7548999999999</v>
+        <v>6203.9503999999997</v>
       </c>
       <c r="K1264" s="13"/>
       <c r="L1264" s="13"/>
       <c r="M1264" s="13"/>
       <c r="N1264" s="15">
-        <v>44614.0527</v>
+        <v>48524.207999999999</v>
       </c>
     </row>
     <row r="1265" spans="1:14" ht="15.75" customHeight="1">
@@ -57566,34 +57565,69 @@
         <v>46053</v>
       </c>
       <c r="B1265" s="22">
-        <v>39309.172100000003</v>
+        <v>63544.9035</v>
       </c>
       <c r="C1265" s="22">
-        <v>6946.4452000000001</v>
+        <v>11986.8099</v>
       </c>
       <c r="D1265" s="22">
-        <v>5658.8904062757165</v>
+        <v>5301.2356106523384</v>
       </c>
       <c r="E1265" s="23">
-        <v>5394.1002568499107</v>
+        <v>5338.0279686621116</v>
       </c>
       <c r="F1265" s="22">
-        <v>957.96249999999998</v>
+        <v>2355.1970000000001</v>
       </c>
       <c r="G1265" s="22">
-        <v>146.49180000000001</v>
+        <v>357.86860000000001</v>
       </c>
       <c r="H1265" s="22">
-        <v>6539.3591996275554</v>
+        <v>6581.1781195667909</v>
       </c>
       <c r="I1265" s="23">
-        <v>7081.0976445614751</v>
+        <v>7018.0263396397113</v>
       </c>
       <c r="J1265" s="22">
-        <v>5487.8076000000001</v>
+        <v>7905.6634999999997</v>
       </c>
       <c r="N1265" s="21">
-        <v>45754.942200000005</v>
+        <v>73805.763999999996</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A1266" s="20">
+        <v>46060</v>
+      </c>
+      <c r="B1266" s="22">
+        <v>27609.502400000001</v>
+      </c>
+      <c r="C1266" s="22">
+        <v>4529.1652000000004</v>
+      </c>
+      <c r="D1266" s="22">
+        <v>6095.9362665773378</v>
+      </c>
+      <c r="E1266" s="23">
+        <v>5425.9088811518031</v>
+      </c>
+      <c r="F1266" s="22">
+        <v>1325.7043000000001</v>
+      </c>
+      <c r="G1266" s="22">
+        <v>187.72649999999999</v>
+      </c>
+      <c r="H1266" s="22">
+        <v>7061.8921675948795</v>
+      </c>
+      <c r="I1266" s="23">
+        <v>7010.4934567378878</v>
+      </c>
+      <c r="J1266" s="22">
+        <v>4703.2345999999998</v>
+      </c>
+      <c r="N1266" s="21">
+        <v>33638.441299999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>